<commit_message>
OK post user (without EntityMAnager.refresh)
</commit_message>
<xml_diff>
--- a/back.xlsx
+++ b/back.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\FP\Factoria F5\Bootcamp fullstack\Proyecto final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A5DE225-72D8-413C-B954-894007FA2AC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1EDC43-F91D-41D5-88BA-74C02F0AA333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30885" yWindow="2430" windowWidth="25275" windowHeight="11385" xr2:uid="{4DAC6932-8D50-40FA-B5DB-9443F4B0FC54}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="57">
   <si>
     <t>Controlador</t>
   </si>
@@ -164,10 +164,49 @@
     <t>List&lt;LogModel&gt;</t>
   </si>
   <si>
-    <t>getAllLogsFromRequest</t>
-  </si>
-  <si>
     <t>findAllByRequestId</t>
+  </si>
+  <si>
+    <t>updateSchool</t>
+  </si>
+  <si>
+    <t>SchoolModel, long</t>
+  </si>
+  <si>
+    <t>deleteSchool</t>
+  </si>
+  <si>
+    <t>deleteLog</t>
+  </si>
+  <si>
+    <t>getAllLogsFromRequestId</t>
+  </si>
+  <si>
+    <t>createLog</t>
+  </si>
+  <si>
+    <t>LogModel</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>updateRequest</t>
+  </si>
+  <si>
+    <t>UserRequestModel, long</t>
+  </si>
+  <si>
+    <t>deleteUSer</t>
+  </si>
+  <si>
+    <t>long id</t>
+  </si>
+  <si>
+    <t>upgradeUser</t>
+  </si>
+  <si>
+    <t>UserModel, long</t>
   </si>
 </sst>
 </file>
@@ -191,7 +230,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -279,15 +318,112 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -297,95 +433,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -702,553 +784,658 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E627246D-9D36-4EDE-BD38-5181D4CF1D58}">
-  <dimension ref="A1:N22"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15:M17"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="24" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="5.140625" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="23.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="25.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.28515625" style="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.28515625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="2" t="s">
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="4"/>
-      <c r="L1" s="18" t="s">
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="24"/>
+      <c r="L1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="16" t="s">
+      <c r="N1" s="8" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="M2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="8" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="24"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
-      <c r="J3" s="24"/>
-      <c r="L3" s="18" t="s">
+      <c r="F3" s="11"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="11"/>
+      <c r="L3" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="M3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="16" t="s">
+      <c r="N3" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
-      <c r="B4" s="6" t="s">
+      <c r="A4" s="29"/>
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="22"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="27"/>
-      <c r="L4" s="18" t="s">
+      <c r="E4" s="36"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="14"/>
+      <c r="L4" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="7" t="s">
+      <c r="M4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="N4" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="29"/>
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E5" s="22"/>
-      <c r="F5" s="27" t="s">
+      <c r="E5" s="36"/>
+      <c r="F5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="28"/>
-      <c r="H5" s="29"/>
-      <c r="I5" s="29"/>
-      <c r="J5" s="27"/>
-      <c r="L5" s="18" t="s">
+      <c r="G5" s="15"/>
+      <c r="H5" s="16"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="14"/>
+      <c r="L5" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="M5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="N5" s="16" t="s">
+      <c r="N5" s="8" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="29"/>
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="27"/>
-      <c r="L6" s="20" t="s">
+      <c r="C6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="14"/>
+      <c r="L6" s="9" t="s">
         <v>27</v>
       </c>
       <c r="M6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="N6" s="17" t="s">
+      <c r="N6" s="8" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="15"/>
-      <c r="B7" s="9" t="s">
+      <c r="A7" s="30"/>
+      <c r="B7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="30"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="30"/>
+      <c r="C7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="37"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="17"/>
+      <c r="L7" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N7" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="24"/>
-      <c r="L8" s="20" t="s">
+      <c r="F8" s="11"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="11"/>
+      <c r="L8" s="9" t="s">
         <v>23</v>
       </c>
       <c r="M8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N8" s="17" t="s">
+      <c r="N8" s="8" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="29"/>
+      <c r="B9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="22"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="29"/>
-      <c r="I9" s="29"/>
-      <c r="J9" s="27"/>
-      <c r="L9" s="20" t="s">
+      <c r="E9" s="36"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="14"/>
+      <c r="L9" s="9" t="s">
         <v>32</v>
       </c>
       <c r="M9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N9" s="17" t="s">
+      <c r="N9" s="8" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="29"/>
+      <c r="B10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="27" t="s">
+      <c r="E10" s="36"/>
+      <c r="F10" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="29"/>
-      <c r="I10" s="29"/>
-      <c r="J10" s="27"/>
-      <c r="L10" s="20" t="s">
+      <c r="G10" s="15"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="14"/>
+      <c r="L10" s="9" t="s">
         <v>24</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N10" s="17" t="s">
+      <c r="N10" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="29"/>
+      <c r="B11" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="29"/>
-      <c r="I11" s="29"/>
-      <c r="J11" s="27"/>
-      <c r="L11" s="20" t="s">
+      <c r="C11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="36"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="14"/>
+      <c r="L11" s="9" t="s">
         <v>37</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="N11" s="17" t="s">
+      <c r="N11" s="8" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="15"/>
-      <c r="B12" s="35" t="s">
+      <c r="A12" s="30"/>
+      <c r="B12" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="30"/>
-      <c r="L12" s="20" t="s">
+      <c r="C12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E12" s="37"/>
+      <c r="F12" s="17"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="19"/>
+      <c r="I12" s="19"/>
+      <c r="J12" s="17"/>
+      <c r="L12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="M12" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="N12" s="17" t="s">
+      <c r="N12" s="33" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="34" t="s">
+      <c r="B13" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="33">
-        <v>0.9</v>
-      </c>
-      <c r="J13" s="24"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="27"/>
+      <c r="J13" s="11"/>
+      <c r="L13" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="M13" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="N13" s="33" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
-      <c r="B14" s="7" t="s">
+      <c r="A14" s="29"/>
+      <c r="B14" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="22"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="22"/>
-      <c r="J14" s="27"/>
-      <c r="L14" s="20" t="s">
+      <c r="E14" s="36"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="16"/>
+      <c r="I14" s="25"/>
+      <c r="J14" s="14"/>
+      <c r="L14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="M14" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="N14" s="17" t="s">
+      <c r="N14" s="33" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
-      <c r="B15" s="7" t="s">
+      <c r="A15" s="29"/>
+      <c r="B15" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="22"/>
-      <c r="F15" s="27" t="s">
+      <c r="E15" s="36"/>
+      <c r="F15" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="28"/>
-      <c r="H15" s="29"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="27"/>
-      <c r="L15" s="18" t="s">
+      <c r="G15" s="15"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="25"/>
+      <c r="J15" s="14"/>
+      <c r="L15" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="M15" s="6" t="s">
+      <c r="M15" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="N15" s="33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="29"/>
+      <c r="B16" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="36"/>
+      <c r="F16" s="14"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="25"/>
+      <c r="J16" s="14"/>
+      <c r="L16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="N16" s="33" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="30"/>
+      <c r="B17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="37"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="19"/>
+      <c r="I17" s="26"/>
+      <c r="J17" s="17"/>
+      <c r="M17" s="32"/>
+      <c r="N17" s="33"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" s="11"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="11"/>
+      <c r="L18" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="N15" s="17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
-      <c r="B16" s="7" t="s">
+      <c r="N18" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="29"/>
+      <c r="B19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E19" s="36"/>
+      <c r="F19" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="15"/>
+      <c r="H19" s="16"/>
+      <c r="I19" s="16"/>
+      <c r="J19" s="14"/>
+      <c r="L19" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="M19" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="N19" s="33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="29"/>
+      <c r="B20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="36"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="14"/>
+      <c r="L20" s="31"/>
+      <c r="M20" s="32"/>
+      <c r="N20" s="33"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="29"/>
+      <c r="B21" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="29"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="27"/>
-      <c r="L16" s="18" t="s">
+      <c r="C21" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D21" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="36"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="14"/>
+      <c r="L21" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="M16" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="N16" s="17" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
-      <c r="B17" s="35" t="s">
+      <c r="M21" s="32" t="s">
+        <v>46</v>
+      </c>
+      <c r="N21" s="33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="30"/>
+      <c r="B22" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="31"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="30"/>
-      <c r="L17" s="18"/>
-      <c r="M17" s="6"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="12"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="24"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
-      <c r="B19" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E19" s="6"/>
-      <c r="F19" s="27" t="s">
-        <v>43</v>
-      </c>
-      <c r="G19" s="28"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="27"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
-      <c r="B20" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="27"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
-      <c r="B21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="27"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="15"/>
-      <c r="B22" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="31"/>
-      <c r="H22" s="32"/>
-      <c r="I22" s="32"/>
-      <c r="J22" s="30"/>
+      <c r="C22" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="37"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="17"/>
+      <c r="L22" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="M22" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="N22" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L23" s="31" t="s">
+        <v>52</v>
+      </c>
+      <c r="M23" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A3:A7"/>
+    <mergeCell ref="A8:A12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="E18:E22"/>
     <mergeCell ref="C1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="E13:E17"/>
     <mergeCell ref="I13:I17"/>
     <mergeCell ref="E3:E7"/>
     <mergeCell ref="E8:E12"/>
-    <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A12"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A18:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>